<commit_message>
update complete project, refactoring files, adding complete old version to not_maintained folder
</commit_message>
<xml_diff>
--- a/test_env/database_creation/rawdata/emissions/all_engines_for_calibration_years.xlsx
+++ b/test_env/database_creation/rawdata/emissions/all_engines_for_calibration_years.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PRohr\Desktop\Masterarbeit\Python\test_env\database_creation\rawdata\emissions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71866139-E057-47E1-B908-EBEE08445A53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D67FEE-146A-42EE-9D55-FA98AD083047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-75" yWindow="0" windowWidth="9750" windowHeight="10155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$6:$E$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$6:$F$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="91">
   <si>
     <t>Engine</t>
   </si>
@@ -152,18 +152,12 @@
     <t>CFM56-7B24</t>
   </si>
   <si>
-    <t>FJR710</t>
-  </si>
-  <si>
     <t>GE90-76B</t>
   </si>
   <si>
     <t>GE90-85B</t>
   </si>
   <si>
-    <t>HFX20</t>
-  </si>
-  <si>
     <t>JT8D-11</t>
   </si>
   <si>
@@ -275,12 +269,6 @@
     <t>only found for JTDP-59A. Might be duplicate</t>
   </si>
   <si>
-    <t>un-verified source: https://saemobilus.sae.org/content/740809/</t>
-  </si>
-  <si>
-    <t>un-verified source: https://hondanews.com/en-US/releases/honda-aero-inc-hai-fact-sheet?l=en-US&amp;mode=print</t>
-  </si>
-  <si>
     <t>Key:</t>
   </si>
   <si>
@@ -318,6 +306,9 @@
   </si>
   <si>
     <t>BR715-55</t>
+  </si>
+  <si>
+    <t>Application Date</t>
   </si>
 </sst>
 </file>
@@ -723,10 +714,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F82"/>
+  <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="68" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E81" sqref="E81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -735,34 +726,35 @@
     <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.31640625" customWidth="1"/>
     <col min="4" max="4" width="11.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.04296875" customWidth="1"/>
-    <col min="6" max="6" width="39.54296875" customWidth="1"/>
+    <col min="5" max="5" width="11.86328125" customWidth="1"/>
+    <col min="6" max="6" width="12.04296875" customWidth="1"/>
+    <col min="7" max="7" width="39.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.75">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A2" s="2"/>
       <c r="B2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.75">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A3" s="4"/>
       <c r="B3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A4" s="3"/>
       <c r="B4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.75">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -773,13 +765,16 @@
         <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.75">
+        <v>90</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -792,13 +787,16 @@
       <c r="D7" s="2">
         <v>1981</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="2">
+        <v>1968</v>
+      </c>
+      <c r="F7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A8" s="1" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A8" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="B8">
         <v>17.600000000000001</v>
@@ -809,11 +807,14 @@
       <c r="D8" s="2">
         <v>1998</v>
       </c>
-      <c r="E8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="E8" s="2">
+        <v>1995</v>
+      </c>
+      <c r="F8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -826,11 +827,14 @@
       <c r="D9" s="2">
         <v>1995</v>
       </c>
-      <c r="E9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="E9" s="2">
+        <v>1993</v>
+      </c>
+      <c r="F9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -843,11 +847,14 @@
       <c r="D10" s="2">
         <v>1977</v>
       </c>
-      <c r="E10" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="E10" s="2">
+        <v>1976</v>
+      </c>
+      <c r="F10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -860,11 +867,14 @@
       <c r="D11" s="2">
         <v>1978</v>
       </c>
-      <c r="E11" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="E11" s="2">
+        <v>1978</v>
+      </c>
+      <c r="F11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -877,11 +887,14 @@
       <c r="D12" s="2">
         <v>1973</v>
       </c>
-      <c r="E12" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="E12" s="2">
+        <v>1971</v>
+      </c>
+      <c r="F12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -894,11 +907,14 @@
       <c r="D13" s="2">
         <v>1976</v>
       </c>
-      <c r="E13" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="E13" s="2">
+        <v>1976</v>
+      </c>
+      <c r="F13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
@@ -911,11 +927,14 @@
       <c r="D14" s="2">
         <v>1978</v>
       </c>
-      <c r="E14" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="E14" s="2">
+        <v>1978</v>
+      </c>
+      <c r="F14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -928,11 +947,14 @@
       <c r="D15" s="2">
         <v>1979</v>
       </c>
-      <c r="E15" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="E15" s="2">
+        <v>1979</v>
+      </c>
+      <c r="F15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
@@ -945,11 +967,14 @@
       <c r="D16" s="2">
         <v>1973</v>
       </c>
-      <c r="E16" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="E16" s="2">
+        <v>1973</v>
+      </c>
+      <c r="F16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A17" s="1" t="s">
         <v>12</v>
       </c>
@@ -962,11 +987,14 @@
       <c r="D17" s="2">
         <v>1975</v>
       </c>
-      <c r="E17" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="E17" s="2">
+        <v>1975</v>
+      </c>
+      <c r="F17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
@@ -979,11 +1007,14 @@
       <c r="D18" s="2">
         <v>1978</v>
       </c>
-      <c r="E18" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="E18" s="2">
+        <v>1978</v>
+      </c>
+      <c r="F18" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A19" s="1" t="s">
         <v>14</v>
       </c>
@@ -996,11 +1027,14 @@
       <c r="D19" s="2">
         <v>1979</v>
       </c>
-      <c r="E19" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="E19" s="2">
+        <v>1979</v>
+      </c>
+      <c r="F19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A20" s="1" t="s">
         <v>15</v>
       </c>
@@ -1013,11 +1047,14 @@
       <c r="D20" s="2">
         <v>1970</v>
       </c>
-      <c r="E20" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="E20" s="2">
+        <v>1968</v>
+      </c>
+      <c r="F20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
@@ -1030,11 +1067,14 @@
       <c r="D21" s="2">
         <v>1978</v>
       </c>
-      <c r="E21" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="E21" s="2">
+        <v>1978</v>
+      </c>
+      <c r="F21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A22" s="1" t="s">
         <v>17</v>
       </c>
@@ -1047,11 +1087,14 @@
       <c r="D22" s="4">
         <v>1993</v>
       </c>
-      <c r="E22" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="E22" s="4">
+        <v>1978</v>
+      </c>
+      <c r="F22" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A23" s="1" t="s">
         <v>18</v>
       </c>
@@ -1064,11 +1107,14 @@
       <c r="D23" s="4">
         <v>1982</v>
       </c>
-      <c r="E23" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="E23" s="4">
+        <v>1980</v>
+      </c>
+      <c r="F23" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A24" s="1" t="s">
         <v>19</v>
       </c>
@@ -1081,11 +1127,14 @@
       <c r="D24" s="4">
         <v>1993</v>
       </c>
-      <c r="E24" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="E24" s="4">
+        <v>1981</v>
+      </c>
+      <c r="F24" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A25" s="1" t="s">
         <v>20</v>
       </c>
@@ -1098,11 +1147,14 @@
       <c r="D25" s="4">
         <v>1982</v>
       </c>
-      <c r="E25" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="E25" s="4">
+        <v>1981</v>
+      </c>
+      <c r="F25" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A26" s="1" t="s">
         <v>21</v>
       </c>
@@ -1115,11 +1167,14 @@
       <c r="D26" s="4">
         <v>1985</v>
       </c>
-      <c r="E26" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="E26" s="4">
+        <v>1984</v>
+      </c>
+      <c r="F26" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A27" s="1" t="s">
         <v>22</v>
       </c>
@@ -1132,11 +1187,14 @@
       <c r="D27" s="4">
         <v>1986</v>
       </c>
-      <c r="E27" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="E27" s="4">
+        <v>1984</v>
+      </c>
+      <c r="F27" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A28" s="1" t="s">
         <v>23</v>
       </c>
@@ -1149,11 +1207,14 @@
       <c r="D28" s="4">
         <v>1987</v>
       </c>
-      <c r="E28" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="E28" s="4">
+        <v>1986</v>
+      </c>
+      <c r="F28" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A29" s="1" t="s">
         <v>24</v>
       </c>
@@ -1166,11 +1227,14 @@
       <c r="D29" s="4">
         <v>1987</v>
       </c>
-      <c r="E29" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="E29" s="4">
+        <v>1984</v>
+      </c>
+      <c r="F29" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A30" s="1" t="s">
         <v>25</v>
       </c>
@@ -1183,11 +1247,14 @@
       <c r="D30" s="4">
         <v>1989</v>
       </c>
-      <c r="E30" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="E30" s="4">
+        <v>1987</v>
+      </c>
+      <c r="F30" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A31" s="1" t="s">
         <v>26</v>
       </c>
@@ -1200,11 +1267,14 @@
       <c r="D31" s="4">
         <v>1987</v>
       </c>
-      <c r="E31" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="E31" s="4">
+        <v>1986</v>
+      </c>
+      <c r="F31" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A32" s="1" t="s">
         <v>27</v>
       </c>
@@ -1217,11 +1287,14 @@
       <c r="D32" s="4">
         <v>1993</v>
       </c>
-      <c r="E32" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="E32" s="4">
+        <v>1991</v>
+      </c>
+      <c r="F32" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A33" s="1" t="s">
         <v>28</v>
       </c>
@@ -1234,14 +1307,17 @@
       <c r="D33" s="3">
         <v>1993</v>
       </c>
-      <c r="E33" t="s">
-        <v>89</v>
+      <c r="E33" s="3">
+        <v>1990</v>
       </c>
       <c r="F33" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.75">
+        <v>85</v>
+      </c>
+      <c r="G33" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A34" s="1" t="s">
         <v>29</v>
       </c>
@@ -1254,11 +1330,14 @@
       <c r="D34" s="4">
         <v>1990</v>
       </c>
-      <c r="E34" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="E34" s="4">
+        <v>1988</v>
+      </c>
+      <c r="F34" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A35" s="1" t="s">
         <v>30</v>
       </c>
@@ -1271,11 +1350,14 @@
       <c r="D35" s="4">
         <v>1994</v>
       </c>
-      <c r="E35" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="E35" s="4">
+        <v>1990</v>
+      </c>
+      <c r="F35" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A36" s="1" t="s">
         <v>31</v>
       </c>
@@ -1288,11 +1370,14 @@
       <c r="D36" s="4">
         <v>1993</v>
       </c>
-      <c r="E36" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="E36" s="4">
+        <v>1990</v>
+      </c>
+      <c r="F36" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A37" s="1" t="s">
         <v>32</v>
       </c>
@@ -1305,11 +1390,14 @@
       <c r="D37" s="4">
         <v>1994</v>
       </c>
-      <c r="E37" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="E37" s="4">
+        <v>1992</v>
+      </c>
+      <c r="F37" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A38" s="1" t="s">
         <v>33</v>
       </c>
@@ -1322,11 +1410,14 @@
       <c r="D38" s="4">
         <v>1991</v>
       </c>
-      <c r="E38" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="E38" s="4">
+        <v>1988</v>
+      </c>
+      <c r="F38" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A39" s="1" t="s">
         <v>34</v>
       </c>
@@ -1339,11 +1430,14 @@
       <c r="D39" s="4">
         <v>1991</v>
       </c>
-      <c r="E39" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="E39" s="4">
+        <v>1988</v>
+      </c>
+      <c r="F39" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A40" s="1" t="s">
         <v>35</v>
       </c>
@@ -1356,11 +1450,14 @@
       <c r="D40" s="4">
         <v>1994</v>
       </c>
-      <c r="E40" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="E40" s="4">
+        <v>1993</v>
+      </c>
+      <c r="F40" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A41" s="1" t="s">
         <v>36</v>
       </c>
@@ -1373,11 +1470,14 @@
       <c r="D41" s="4">
         <v>1996</v>
       </c>
-      <c r="E41" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="E41" s="4">
+        <v>1994</v>
+      </c>
+      <c r="F41" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A42" s="1" t="s">
         <v>37</v>
       </c>
@@ -1390,377 +1490,437 @@
       <c r="D42" s="4">
         <v>1996</v>
       </c>
-      <c r="E42" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="E42" s="4">
+        <v>1994</v>
+      </c>
+      <c r="F42" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A43" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B43">
-        <v>19.3</v>
+        <v>15.4</v>
       </c>
       <c r="C43">
-        <v>10.6</v>
-      </c>
-      <c r="D43" s="3">
-        <v>1971</v>
-      </c>
-      <c r="E43" t="s">
-        <v>89</v>
+        <v>7.7204724409448833</v>
+      </c>
+      <c r="D43" s="4">
+        <v>1995</v>
+      </c>
+      <c r="E43" s="4">
+        <v>1991</v>
       </c>
       <c r="F43" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.75">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A44" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B44">
-        <v>15.4</v>
+        <v>14.7</v>
       </c>
       <c r="C44">
-        <v>7.7204724409448833</v>
+        <v>7.9036605322121796</v>
       </c>
       <c r="D44" s="4">
         <v>1995</v>
       </c>
-      <c r="E44" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="E44" s="4">
+        <v>1991</v>
+      </c>
+      <c r="F44" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A45" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45">
+        <v>22.6</v>
+      </c>
+      <c r="C45">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="D45" s="2">
+        <v>1966</v>
+      </c>
+      <c r="E45" s="2">
+        <v>1966</v>
+      </c>
+      <c r="F45" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A46" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B45">
-        <v>14.7</v>
-      </c>
-      <c r="C45">
-        <v>7.9036605322121796</v>
-      </c>
-      <c r="D45" s="4">
-        <v>1995</v>
-      </c>
-      <c r="E45" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.75">
-      <c r="A46" s="1" t="s">
+      <c r="B46">
+        <v>22.8</v>
+      </c>
+      <c r="C46">
+        <v>16.88687050359712</v>
+      </c>
+      <c r="D46" s="2">
+        <v>1968</v>
+      </c>
+      <c r="E46" s="2">
+        <v>1968</v>
+      </c>
+      <c r="F46" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A47" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B46">
-        <v>21.87</v>
-      </c>
-      <c r="C46">
-        <v>12.5</v>
-      </c>
-      <c r="D46" s="3">
-        <v>1996</v>
-      </c>
-      <c r="E46" t="s">
-        <v>89</v>
-      </c>
-      <c r="F46" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.75">
-      <c r="A47" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="B47">
-        <v>22.6</v>
+        <v>22.934999999999999</v>
       </c>
       <c r="C47">
-        <v>16.600000000000001</v>
+        <v>17.254493762692199</v>
       </c>
       <c r="D47" s="2">
-        <v>1966</v>
-      </c>
-      <c r="E47" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.75">
+        <v>1971</v>
+      </c>
+      <c r="E47" s="2">
+        <v>1969</v>
+      </c>
+      <c r="F47" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A48" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B48">
-        <v>22.8</v>
+        <v>22.9</v>
       </c>
       <c r="C48">
-        <v>16.88687050359712</v>
+        <v>16.2535683202785</v>
       </c>
       <c r="D48" s="2">
-        <v>1968</v>
-      </c>
-      <c r="E48" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.75">
+        <v>1982</v>
+      </c>
+      <c r="E48" s="2">
+        <v>1980</v>
+      </c>
+      <c r="F48" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A49" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B49">
-        <v>22.934999999999999</v>
+        <v>23.234999999999999</v>
       </c>
       <c r="C49">
-        <v>17.254493762692199</v>
+        <v>18.05903821835043</v>
       </c>
       <c r="D49" s="2">
-        <v>1971</v>
-      </c>
-      <c r="E49" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.75">
+        <v>1974</v>
+      </c>
+      <c r="E49" s="2">
+        <v>1973</v>
+      </c>
+      <c r="F49" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A50" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B50">
-        <v>22.9</v>
+        <v>21.9</v>
       </c>
       <c r="C50">
-        <v>16.2535683202785</v>
+        <v>16.554166081213999</v>
       </c>
       <c r="D50" s="2">
         <v>1982</v>
       </c>
-      <c r="E50" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="E50" s="2">
+        <v>1980</v>
+      </c>
+      <c r="F50" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A51" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B51">
-        <v>23.234999999999999</v>
+        <v>22.1</v>
       </c>
       <c r="C51">
-        <v>18.05903821835043</v>
+        <v>17.693748385430119</v>
       </c>
       <c r="D51" s="2">
-        <v>1974</v>
-      </c>
-      <c r="E51" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.75">
+        <v>1983</v>
+      </c>
+      <c r="E51" s="2">
+        <v>1980</v>
+      </c>
+      <c r="F51" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A52" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B52">
-        <v>21.9</v>
+        <v>23.2</v>
       </c>
       <c r="C52">
-        <v>16.554166081213999</v>
+        <v>18.371738568845259</v>
       </c>
       <c r="D52" s="2">
-        <v>1982</v>
-      </c>
-      <c r="E52" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.75">
+        <v>1976</v>
+      </c>
+      <c r="E52" s="2">
+        <v>1974</v>
+      </c>
+      <c r="F52" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A53" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B53">
-        <v>22.1</v>
+        <v>20.5</v>
       </c>
       <c r="C53">
-        <v>17.693748385430119</v>
+        <v>13.957932242990649</v>
       </c>
       <c r="D53" s="2">
-        <v>1983</v>
-      </c>
-      <c r="E53" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.75">
+        <v>1979</v>
+      </c>
+      <c r="E53" s="2">
+        <v>1977</v>
+      </c>
+      <c r="F53" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A54" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B54">
-        <v>23.2</v>
+        <v>21.3</v>
       </c>
       <c r="C54">
-        <v>18.371738568845259</v>
+        <v>14.27547983610093</v>
       </c>
       <c r="D54" s="2">
-        <v>1976</v>
-      </c>
-      <c r="E54" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.75">
+        <v>1980</v>
+      </c>
+      <c r="E54" s="2">
+        <v>1978</v>
+      </c>
+      <c r="F54" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A55" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B55">
-        <v>20.5</v>
+        <v>21.3</v>
       </c>
       <c r="C55">
-        <v>13.957932242990649</v>
+        <v>14.27547983610093</v>
       </c>
       <c r="D55" s="2">
-        <v>1979</v>
-      </c>
-      <c r="E55" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.75">
+        <v>1981</v>
+      </c>
+      <c r="E55" s="2">
+        <v>1981</v>
+      </c>
+      <c r="F55" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A56" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B56">
-        <v>21.3</v>
+        <v>20.8</v>
       </c>
       <c r="C56">
-        <v>14.27547983610093</v>
+        <v>13.87222342031486</v>
       </c>
       <c r="D56" s="2">
-        <v>1980</v>
-      </c>
-      <c r="E56" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.75">
+        <v>1986</v>
+      </c>
+      <c r="E56" s="2">
+        <v>1985</v>
+      </c>
+      <c r="F56" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A57" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B57">
-        <v>21.3</v>
+        <v>20.9</v>
       </c>
       <c r="C57">
-        <v>14.27547983610093</v>
+        <v>14.0641007045172</v>
       </c>
       <c r="D57" s="2">
-        <v>1981</v>
-      </c>
-      <c r="E57" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.75">
+        <v>1985</v>
+      </c>
+      <c r="E57" s="2">
+        <v>1983</v>
+      </c>
+      <c r="F57" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A58" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B58">
-        <v>20.8</v>
+        <v>22.55</v>
       </c>
       <c r="C58">
-        <v>13.87222342031486</v>
+        <v>16.28745784486912</v>
       </c>
       <c r="D58" s="2">
-        <v>1986</v>
-      </c>
-      <c r="E58" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.75">
+        <v>1966</v>
+      </c>
+      <c r="E58" s="2">
+        <v>1966</v>
+      </c>
+      <c r="F58" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A59" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B59">
-        <v>20.9</v>
+        <v>22.763999999999999</v>
       </c>
       <c r="C59">
-        <v>14.0641007045172</v>
+        <v>16.38183875968992</v>
       </c>
       <c r="D59" s="2">
-        <v>1985</v>
-      </c>
-      <c r="E59" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.75">
+        <v>1967</v>
+      </c>
+      <c r="E59" s="2">
+        <v>1966</v>
+      </c>
+      <c r="F59" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A60" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B60">
-        <v>22.55</v>
+        <v>17.7</v>
       </c>
       <c r="C60">
-        <v>16.28745784486912</v>
+        <v>10.4693345323741</v>
       </c>
       <c r="D60" s="2">
-        <v>1966</v>
-      </c>
-      <c r="E60" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.75">
+        <v>1986</v>
+      </c>
+      <c r="E60" s="2">
+        <v>1986</v>
+      </c>
+      <c r="F60" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A61" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B61">
-        <v>22.763999999999999</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="C61">
-        <v>16.38183875968992</v>
-      </c>
-      <c r="D61" s="2">
-        <v>1967</v>
-      </c>
-      <c r="E61" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.75">
+        <v>10.6</v>
+      </c>
+      <c r="D61" s="3">
+        <v>1974</v>
+      </c>
+      <c r="E61" s="3">
+        <v>1974</v>
+      </c>
+      <c r="F61" t="s">
+        <v>86</v>
+      </c>
+      <c r="G61" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A62" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B62">
-        <v>17.7</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="C62">
-        <v>10.4693345323741</v>
+        <v>10.38528413910093</v>
       </c>
       <c r="D62" s="2">
-        <v>1986</v>
-      </c>
-      <c r="E62" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.75">
+        <v>1974</v>
+      </c>
+      <c r="E62" s="2">
+        <v>1974</v>
+      </c>
+      <c r="F62" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A63" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B63">
-        <v>17.899999999999999</v>
+        <v>22.6</v>
       </c>
       <c r="C63">
-        <v>10.6</v>
-      </c>
-      <c r="D63" s="3">
-        <v>1974</v>
-      </c>
-      <c r="E63" t="s">
-        <v>90</v>
+        <v>16.600000000000001</v>
+      </c>
+      <c r="D63" s="2">
+        <v>1971</v>
+      </c>
+      <c r="E63" s="2">
+        <v>1970</v>
       </c>
       <c r="F63" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.75">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A64" s="1" t="s">
         <v>58</v>
       </c>
@@ -1773,28 +1933,34 @@
       <c r="D64" s="2">
         <v>1974</v>
       </c>
-      <c r="E64" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="E64" s="2">
+        <v>1974</v>
+      </c>
+      <c r="F64" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A65" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B65">
-        <v>22.6</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="C65">
-        <v>16.600000000000001</v>
+        <v>10.15714285714286</v>
       </c>
       <c r="D65" s="2">
-        <v>1971</v>
-      </c>
-      <c r="E65" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.75">
+        <v>1974</v>
+      </c>
+      <c r="E65" s="2">
+        <v>1974</v>
+      </c>
+      <c r="F65" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A66" s="1" t="s">
         <v>60</v>
       </c>
@@ -1802,16 +1968,19 @@
         <v>17.899999999999999</v>
       </c>
       <c r="C66">
-        <v>10.38528413910093</v>
+        <v>10.438669064748201</v>
       </c>
       <c r="D66" s="2">
+        <v>1976</v>
+      </c>
+      <c r="E66" s="2">
         <v>1974</v>
       </c>
-      <c r="E66" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="F66" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A67" s="1" t="s">
         <v>61</v>
       </c>
@@ -1819,229 +1988,268 @@
         <v>17.899999999999999</v>
       </c>
       <c r="C67">
-        <v>10.15714285714286</v>
+        <v>10.38748674443266</v>
       </c>
       <c r="D67" s="2">
-        <v>1974</v>
-      </c>
-      <c r="E67" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.75">
+        <v>1978</v>
+      </c>
+      <c r="E67" s="2">
+        <v>1977</v>
+      </c>
+      <c r="F67" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A68" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B68">
-        <v>17.899999999999999</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="C68">
-        <v>10.438669064748201</v>
-      </c>
-      <c r="D68" s="2">
-        <v>1976</v>
-      </c>
-      <c r="E68" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.75">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="D68" s="3">
+        <v>1980</v>
+      </c>
+      <c r="E68" s="3">
+        <v>1979</v>
+      </c>
+      <c r="F68" t="s">
+        <v>86</v>
+      </c>
+      <c r="G68" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A69" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B69">
-        <v>17.899999999999999</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="C69">
-        <v>10.38748674443266</v>
+        <v>9.9930184804928128</v>
       </c>
       <c r="D69" s="2">
-        <v>1978</v>
-      </c>
-      <c r="E69" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.75">
+        <v>1982</v>
+      </c>
+      <c r="E69" s="2">
+        <v>1979</v>
+      </c>
+      <c r="F69" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A70" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B70">
-        <v>17.399999999999999</v>
+        <v>17.8</v>
       </c>
       <c r="C70">
-        <v>9.6999999999999993</v>
-      </c>
-      <c r="D70" s="3">
-        <v>1980</v>
-      </c>
-      <c r="E70" t="s">
-        <v>90</v>
+        <v>10.10501806503413</v>
+      </c>
+      <c r="D70" s="2">
+        <v>1982</v>
+      </c>
+      <c r="E70" s="2">
+        <v>1979</v>
       </c>
       <c r="F70" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.75">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A71" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B71">
-        <v>18.100000000000001</v>
+        <v>16.5</v>
       </c>
       <c r="C71">
-        <v>9.9930184804928128</v>
+        <v>9.4679110309588239</v>
       </c>
       <c r="D71" s="2">
-        <v>1982</v>
-      </c>
-      <c r="E71" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.75">
+        <v>1983</v>
+      </c>
+      <c r="E71" s="2">
+        <v>1980</v>
+      </c>
+      <c r="F71" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A72" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B72">
-        <v>17.8</v>
+        <v>16.31666666666667</v>
       </c>
       <c r="C72">
-        <v>10.10501806503413</v>
-      </c>
-      <c r="D72" s="2">
-        <v>1982</v>
-      </c>
-      <c r="E72" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.75">
+        <v>9.5454250448668656</v>
+      </c>
+      <c r="D72" s="5">
+        <v>1986</v>
+      </c>
+      <c r="E72" s="5">
+        <v>1986</v>
+      </c>
+      <c r="F72" t="s">
+        <v>86</v>
+      </c>
+      <c r="G72" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A73" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B73">
-        <v>16.5</v>
+        <v>15.95</v>
       </c>
       <c r="C73">
-        <v>9.4679110309588239</v>
-      </c>
-      <c r="D73" s="2">
-        <v>1983</v>
-      </c>
-      <c r="E73" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.75">
+        <v>9.69</v>
+      </c>
+      <c r="D73" s="5">
+        <v>1994</v>
+      </c>
+      <c r="E73" s="5">
+        <v>1994</v>
+      </c>
+      <c r="F73" t="s">
+        <v>85</v>
+      </c>
+      <c r="G73" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A74" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B74">
-        <v>16.31666666666667</v>
+        <v>19.29</v>
       </c>
       <c r="C74">
-        <v>9.5454250448668656</v>
-      </c>
-      <c r="D74" s="5">
-        <v>1986</v>
-      </c>
-      <c r="E74" t="s">
-        <v>90</v>
+        <v>10.99</v>
+      </c>
+      <c r="D74" s="4">
+        <v>1995</v>
+      </c>
+      <c r="E74" s="4">
+        <v>1992</v>
       </c>
       <c r="F74" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.75">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A75" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B75">
-        <v>15.95</v>
+        <v>19.23</v>
       </c>
       <c r="C75">
-        <v>9.69</v>
-      </c>
-      <c r="D75" s="5">
-        <v>1994</v>
-      </c>
-      <c r="E75" t="s">
-        <v>89</v>
+        <v>11.16</v>
+      </c>
+      <c r="D75" s="4">
+        <v>1999</v>
+      </c>
+      <c r="E75" s="4">
+        <v>1998</v>
       </c>
       <c r="F75" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.75">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A76" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B76">
-        <v>19.29</v>
+        <v>23.2</v>
       </c>
       <c r="C76">
-        <v>10.99</v>
-      </c>
-      <c r="D76" s="4">
-        <v>1995</v>
-      </c>
-      <c r="E76" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.75">
+        <v>13.67775757575758</v>
+      </c>
+      <c r="D76" s="2">
+        <v>1974</v>
+      </c>
+      <c r="E76" s="2">
+        <v>1969</v>
+      </c>
+      <c r="F76" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A77" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B77">
-        <v>19.23</v>
+        <v>16.5</v>
       </c>
       <c r="C77">
-        <v>11.16</v>
-      </c>
-      <c r="D77" s="4">
-        <v>1999</v>
-      </c>
-      <c r="E77" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.75">
+        <v>9.9</v>
+      </c>
+      <c r="D77" s="2">
+        <v>1988</v>
+      </c>
+      <c r="E77" s="2">
+        <v>1993</v>
+      </c>
+      <c r="F77" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A78" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B78">
-        <v>23.2</v>
+        <v>16.3</v>
       </c>
       <c r="C78">
-        <v>13.67775757575758</v>
-      </c>
-      <c r="D78" s="2">
-        <v>1974</v>
-      </c>
-      <c r="E78" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.75">
+        <v>9.6</v>
+      </c>
+      <c r="D78" s="4">
+        <v>1996</v>
+      </c>
+      <c r="E78" s="4">
+        <v>1995</v>
+      </c>
+      <c r="F78" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A79" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B79">
-        <v>16.5</v>
+        <v>16.3</v>
       </c>
       <c r="C79">
-        <v>9.9</v>
-      </c>
-      <c r="D79" s="2">
-        <v>1988</v>
-      </c>
-      <c r="E79" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.75">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="D79" s="4">
+        <v>1993</v>
+      </c>
+      <c r="E79" s="4">
+        <v>1993</v>
+      </c>
+      <c r="F79" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A80" s="1" t="s">
         <v>74</v>
       </c>
@@ -2049,51 +2257,20 @@
         <v>16.3</v>
       </c>
       <c r="C80">
-        <v>9.6</v>
+        <v>10.5</v>
       </c>
       <c r="D80" s="4">
+        <v>1997</v>
+      </c>
+      <c r="E80" s="4">
         <v>1996</v>
       </c>
-      <c r="E80" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A81" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B81">
-        <v>16.3</v>
-      </c>
-      <c r="C81">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="D81" s="4">
-        <v>1993</v>
-      </c>
-      <c r="E81" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A82" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B82">
-        <v>16.3</v>
-      </c>
-      <c r="C82">
-        <v>10.5</v>
-      </c>
-      <c r="D82" s="4">
-        <v>1997</v>
-      </c>
-      <c r="E82" t="s">
-        <v>90</v>
+      <c r="F80" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A6:E6" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A6:F6" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
add some payload range statistics
</commit_message>
<xml_diff>
--- a/test_env/database_creation/rawdata/emissions/all_engines_for_calibration_years.xlsx
+++ b/test_env/database_creation/rawdata/emissions/all_engines_for_calibration_years.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PRohr\Desktop\Masterarbeit\Python\test_env\database_creation\rawdata\emissions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7547B751-391B-41BC-8CA8-CAC81DAA5997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5036D399-15E2-42BD-BC30-20E492ADBF5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-75" yWindow="0" windowWidth="9750" windowHeight="10155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-21710" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="154">
   <si>
     <t>Engine</t>
   </si>
@@ -423,6 +423,81 @@
   </si>
   <si>
     <t>Ukraine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Newer Engines found: </t>
+  </si>
+  <si>
+    <t>Leap 1A</t>
+  </si>
+  <si>
+    <t>Leap 1B</t>
+  </si>
+  <si>
+    <t>Leap 1C</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/CFM_International_LEAP#Specifications</t>
+  </si>
+  <si>
+    <t>Not sure is source reliable, some russian blog</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Trent XWB-97</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Rolls-Royce_Trent_XWB#Specifications</t>
+  </si>
+  <si>
+    <t>No source given</t>
+  </si>
+  <si>
+    <t>Trent 900</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Rolls-Royce_Trent_900#Specifications_(Trent_900)</t>
+  </si>
+  <si>
+    <t>Icao Cal</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>15.37-15.44</t>
+  </si>
+  <si>
+    <t>14.76-15.14</t>
+  </si>
+  <si>
+    <t>15.39-15.86</t>
+  </si>
+  <si>
+    <t>notfound</t>
+  </si>
+  <si>
+    <t>14.97-15.66</t>
+  </si>
+  <si>
+    <t>2.5-5.1%</t>
+  </si>
+  <si>
+    <t>, -4- -3.5%</t>
+  </si>
+  <si>
+    <t>10.9-15.5%</t>
+  </si>
+  <si>
+    <t>2.6-5.7%</t>
+  </si>
+  <si>
+    <t>How reliable is this data?</t>
   </si>
 </sst>
 </file>
@@ -600,7 +675,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -622,6 +697,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -925,10 +1001,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I108"/>
+  <dimension ref="A1:N108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A97" sqref="A97"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -940,33 +1016,33 @@
     <col min="5" max="5" width="11.86328125" customWidth="1"/>
     <col min="6" max="6" width="12.04296875" customWidth="1"/>
     <col min="7" max="7" width="39.54296875" customWidth="1"/>
-    <col min="9" max="9" width="95" customWidth="1"/>
+    <col min="9" max="9" width="16.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A2" s="2"/>
       <c r="B2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A3" s="4"/>
       <c r="B3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="4" spans="1:14" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A4" s="3"/>
       <c r="B4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="5" spans="1:14" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="H5" s="11" t="s">
         <v>84</v>
       </c>
@@ -974,7 +1050,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -1001,7 +1077,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -1027,7 +1103,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A8" s="1" t="s">
         <v>89</v>
       </c>
@@ -1053,7 +1129,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -1079,7 +1155,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="10" spans="1:14" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -1105,7 +1181,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -1125,7 +1201,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -1145,7 +1221,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -1164,8 +1240,26 @@
       <c r="F13" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="H13" t="s">
+        <v>129</v>
+      </c>
+      <c r="I13" t="s">
+        <v>133</v>
+      </c>
+      <c r="J13" t="s">
+        <v>142</v>
+      </c>
+      <c r="K13" t="s">
+        <v>143</v>
+      </c>
+      <c r="M13" t="s">
+        <v>84</v>
+      </c>
+      <c r="N13" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
@@ -1184,8 +1278,26 @@
       <c r="F14" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="H14" t="s">
+        <v>130</v>
+      </c>
+      <c r="I14">
+        <v>14.4</v>
+      </c>
+      <c r="J14" t="s">
+        <v>145</v>
+      </c>
+      <c r="K14" t="s">
+        <v>149</v>
+      </c>
+      <c r="M14" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="N14" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -1204,8 +1316,26 @@
       <c r="F15" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="H15" t="s">
+        <v>131</v>
+      </c>
+      <c r="I15">
+        <v>15</v>
+      </c>
+      <c r="J15" t="s">
+        <v>146</v>
+      </c>
+      <c r="K15" t="s">
+        <v>152</v>
+      </c>
+      <c r="M15" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="N15" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
@@ -1224,8 +1354,23 @@
       <c r="F16" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="H16" t="s">
+        <v>132</v>
+      </c>
+      <c r="I16">
+        <v>14.4</v>
+      </c>
+      <c r="J16" t="s">
+        <v>147</v>
+      </c>
+      <c r="M16" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="N16" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A17" s="1" t="s">
         <v>12</v>
       </c>
@@ -1244,8 +1389,26 @@
       <c r="F17" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="H17" t="s">
+        <v>137</v>
+      </c>
+      <c r="I17">
+        <v>13.5</v>
+      </c>
+      <c r="J17" t="s">
+        <v>148</v>
+      </c>
+      <c r="K17" t="s">
+        <v>151</v>
+      </c>
+      <c r="M17" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="N17" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
@@ -1264,8 +1427,26 @@
       <c r="F18" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="H18" t="s">
+        <v>140</v>
+      </c>
+      <c r="I18">
+        <v>16</v>
+      </c>
+      <c r="J18" t="s">
+        <v>144</v>
+      </c>
+      <c r="K18" t="s">
+        <v>150</v>
+      </c>
+      <c r="M18" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="N18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A19" s="1" t="s">
         <v>14</v>
       </c>
@@ -1285,7 +1466,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A20" s="1" t="s">
         <v>15</v>
       </c>
@@ -1305,7 +1486,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
@@ -1324,8 +1505,11 @@
       <c r="F21" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="N21" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A22" s="1" t="s">
         <v>17</v>
       </c>
@@ -1345,7 +1529,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A23" s="1" t="s">
         <v>18</v>
       </c>
@@ -1365,7 +1549,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A24" s="1" t="s">
         <v>19</v>
       </c>
@@ -1385,7 +1569,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A25" s="1" t="s">
         <v>20</v>
       </c>
@@ -1405,7 +1589,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A26" s="1" t="s">
         <v>21</v>
       </c>
@@ -1425,7 +1609,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A27" s="1" t="s">
         <v>22</v>
       </c>
@@ -1445,7 +1629,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A28" s="1" t="s">
         <v>23</v>
       </c>
@@ -1465,7 +1649,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A29" s="1" t="s">
         <v>24</v>
       </c>
@@ -1485,7 +1669,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A30" s="1" t="s">
         <v>25</v>
       </c>
@@ -1505,7 +1689,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A31" s="1" t="s">
         <v>26</v>
       </c>
@@ -1525,7 +1709,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A32" s="1" t="s">
         <v>27</v>
       </c>
@@ -2972,8 +3156,13 @@
     <hyperlink ref="I7" r:id="rId3" xr:uid="{1887F211-F955-4C9B-8F85-C87421092B30}"/>
     <hyperlink ref="I8" r:id="rId4" xr:uid="{E2B9A340-24AE-4FB7-82F1-C3F10B25C2EE}"/>
     <hyperlink ref="I10" r:id="rId5" xr:uid="{838081F6-AF7F-4665-9C28-0E5A843747C3}"/>
+    <hyperlink ref="M14" r:id="rId6" location="Specifications" xr:uid="{5B3EECDD-BD42-439E-AD15-13E8C660EAFF}"/>
+    <hyperlink ref="M15" r:id="rId7" location="Specifications" xr:uid="{2E202FA4-9593-4CC6-9E0F-7007FEDF4E7B}"/>
+    <hyperlink ref="M16" r:id="rId8" location="Specifications" xr:uid="{F16BCC41-753A-459C-ACC8-6C7B9FCC05F9}"/>
+    <hyperlink ref="M17" r:id="rId9" location="Specifications" xr:uid="{2D56CC4F-9764-4B6C-933A-15A44305BA32}"/>
+    <hyperlink ref="M18" r:id="rId10" location="Specifications_(Trent_900)" xr:uid="{D0AA59CD-881F-432D-B0F6-8DF24ADEE60E}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>